<commit_message>
start to increase experiences
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="152">
   <si>
     <t>Golisopod</t>
   </si>
@@ -213,12 +213,6 @@
     <t>L44 Learn</t>
   </si>
   <si>
-    <t>L36 Forget Iron Defense</t>
-  </si>
-  <si>
-    <t>L37 Forget Growth</t>
-  </si>
-  <si>
     <t>L51 Learn</t>
   </si>
   <si>
@@ -234,12 +228,6 @@
     <t>50 Forget Destiny Bond</t>
   </si>
   <si>
-    <t>44 Forget Dark Pulse</t>
-  </si>
-  <si>
-    <t>39 Forget Dream Eater</t>
-  </si>
-  <si>
     <t>Ghost/Poison</t>
   </si>
   <si>
@@ -283,6 +271,207 @@
   </si>
   <si>
     <t>Adamant/Sap Sipper</t>
+  </si>
+  <si>
+    <t>L44 Forget Flamethrower</t>
+  </si>
+  <si>
+    <t>L49 Forget Scary</t>
+  </si>
+  <si>
+    <t>L55 Learn Flare Blitz</t>
+  </si>
+  <si>
+    <t>L60 Forget Outrage</t>
+  </si>
+  <si>
+    <t>L66 Forget Cross Chop</t>
+  </si>
+  <si>
+    <t>TM26 Earthquack</t>
+  </si>
+  <si>
+    <t>L42 Forget Counter</t>
+  </si>
+  <si>
+    <t>L47 Learn Earthquack</t>
+  </si>
+  <si>
+    <t>L55 Learn Mega Kick</t>
+  </si>
+  <si>
+    <t>L60 Learn Superpower</t>
+  </si>
+  <si>
+    <t>egg Close Combat</t>
+  </si>
+  <si>
+    <t>L36 Learn Hammer Arm</t>
+  </si>
+  <si>
+    <t>L43 Learn Thrash</t>
+  </si>
+  <si>
+    <t>L49 Forget Pain Split</t>
+  </si>
+  <si>
+    <t>L56 Learn Double Edge 120</t>
+  </si>
+  <si>
+    <t>L62 Learn Superpower 120</t>
+  </si>
+  <si>
+    <t>TM26 Earthquack 100</t>
+  </si>
+  <si>
+    <t>TM68 Giga Impact 150</t>
+  </si>
+  <si>
+    <t>Adamant/Fluffy</t>
+  </si>
+  <si>
+    <t>Quiet/Schooling</t>
+  </si>
+  <si>
+    <t>L41 Learn Double-edge</t>
+  </si>
+  <si>
+    <t>L46 Forget Soak</t>
+  </si>
+  <si>
+    <t>L49 Forget Endeavor</t>
+  </si>
+  <si>
+    <t>L54 Learn Hydro Pump</t>
+  </si>
+  <si>
+    <t>TM13 Ice Beam 90</t>
+  </si>
+  <si>
+    <t>Work Up</t>
+  </si>
+  <si>
+    <t>Echoed Voice</t>
+  </si>
+  <si>
+    <t>Normal/Spec</t>
+  </si>
+  <si>
+    <t>Normal/Status</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Confide</t>
+  </si>
+  <si>
+    <t>Brick Break</t>
+  </si>
+  <si>
+    <t>Fighting/attack</t>
+  </si>
+  <si>
+    <t>Infestation</t>
+  </si>
+  <si>
+    <t>Bug/Spec</t>
+  </si>
+  <si>
+    <t>Acrobatics</t>
+  </si>
+  <si>
+    <t>Flying/attack</t>
+  </si>
+  <si>
+    <t>Charge Beam</t>
+  </si>
+  <si>
+    <t>Electric/Spec</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Dark/attack</t>
+  </si>
+  <si>
+    <t>Fling</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>Torment</t>
+  </si>
+  <si>
+    <t>Dark/status</t>
+  </si>
+  <si>
+    <t>Sleep Talk</t>
+  </si>
+  <si>
+    <t>Normal/status</t>
+  </si>
+  <si>
+    <t>Rest</t>
+  </si>
+  <si>
+    <t>Psychic/status</t>
+  </si>
+  <si>
+    <t>Tock Tomb</t>
+  </si>
+  <si>
+    <t>Rock/attack</t>
+  </si>
+  <si>
+    <t>Flame Charge</t>
+  </si>
+  <si>
+    <t>Fire/attack</t>
+  </si>
+  <si>
+    <t>Sky Drop</t>
+  </si>
+  <si>
+    <t>Nature Power</t>
+  </si>
+  <si>
+    <t>Thunder Wave</t>
+  </si>
+  <si>
+    <t>Grass Knot</t>
+  </si>
+  <si>
+    <t>Grass/Spec</t>
+  </si>
+  <si>
+    <t>Smart Strike</t>
+  </si>
+  <si>
+    <t>Steel/attack</t>
+  </si>
+  <si>
+    <t>Rain Dance</t>
+  </si>
+  <si>
+    <t>Water/status</t>
+  </si>
+  <si>
+    <t>Normal/attack</t>
+  </si>
+  <si>
+    <t>Hidden Power</t>
+  </si>
+  <si>
+    <t>Water/Spec</t>
+  </si>
+  <si>
+    <t>L44 Forget Dark Pulse</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -410,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -436,6 +625,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -755,14 +948,15 @@
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="D1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -779,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>
@@ -794,27 +988,24 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="E3">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>17</v>
@@ -829,19 +1020,16 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>150</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" t="s">
         <v>69</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -893,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>9</v>
@@ -908,24 +1096,21 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" t="s">
         <v>63</v>
       </c>
+      <c r="K5" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="L5" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="N5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="P5" t="s">
+      <c r="O5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -934,7 +1119,7 @@
         <v>530</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -942,10 +1127,10 @@
       <c r="E6">
         <v>39</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="24" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -953,6 +1138,24 @@
       </c>
       <c r="I6" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6" t="s">
+        <v>89</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -966,12 +1169,12 @@
         <v>5</v>
       </c>
       <c r="E7">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="25" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -979,6 +1182,24 @@
       </c>
       <c r="I7" s="9" t="s">
         <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -986,13 +1207,16 @@
         <v>500</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
       <c r="E8">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>29</v>
@@ -1006,10 +1230,31 @@
       <c r="I8" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="J8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="P8" s="15" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -1017,8 +1262,11 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
       <c r="E9">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>31</v>
@@ -1029,8 +1277,26 @@
       <c r="H9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="17" t="s">
         <v>34</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" t="s">
+        <v>106</v>
+      </c>
+      <c r="L9" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="O9" s="26" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1038,10 +1304,10 @@
         <v>500</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
@@ -1053,13 +1319,13 @@
         <v>600</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="5"/>
@@ -1071,10 +1337,10 @@
         <v>530</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D12" s="22"/>
       <c r="F12" s="3"/>
@@ -1087,10 +1353,10 @@
         <v>500</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D13" s="21"/>
       <c r="F13" s="3"/>
@@ -1106,7 +1372,7 @@
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1124,55 +1390,58 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:8">
       <c r="C17" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:8">
       <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:8">
       <c r="C19" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:8">
       <c r="C20" s="7" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:8">
       <c r="C21" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:8">
       <c r="C22" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" spans="3:8">
       <c r="C23" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="3:4">
+      <c r="H23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8">
       <c r="C24" s="9" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="3:4">
+    <row r="25" spans="3:8">
       <c r="C25" s="8" t="s">
         <v>45</v>
       </c>
@@ -1186,12 +1455,441 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31">
+        <v>75</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39">
+        <v>60</v>
+      </c>
+      <c r="D39">
+        <v>95</v>
+      </c>
+      <c r="E39">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43">
+        <v>50</v>
+      </c>
+      <c r="D43">
+        <v>100</v>
+      </c>
+      <c r="E43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46">
+        <v>60</v>
+      </c>
+      <c r="D46">
+        <v>100</v>
+      </c>
+      <c r="E46">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48">
+        <v>60</v>
+      </c>
+      <c r="D48">
+        <v>100</v>
+      </c>
+      <c r="E48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49">
+        <v>40</v>
+      </c>
+      <c r="D49">
+        <v>100</v>
+      </c>
+      <c r="E49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54">
+        <v>40</v>
+      </c>
+      <c r="D54">
+        <v>100</v>
+      </c>
+      <c r="E54">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55">
+        <v>80</v>
+      </c>
+      <c r="D55">
+        <v>100</v>
+      </c>
+      <c r="E55">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" t="s">
+        <v>125</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56">
+        <v>100</v>
+      </c>
+      <c r="E56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57">
+        <v>50</v>
+      </c>
+      <c r="D57">
+        <v>90</v>
+      </c>
+      <c r="E57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58">
+        <v>60</v>
+      </c>
+      <c r="D58">
+        <v>100</v>
+      </c>
+      <c r="E58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59">
+        <v>60</v>
+      </c>
+      <c r="D59">
+        <v>100</v>
+      </c>
+      <c r="E59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62">
+        <v>55</v>
+      </c>
+      <c r="D62">
+        <v>100</v>
+      </c>
+      <c r="E62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67">
+        <v>70</v>
+      </c>
+      <c r="D67" t="s">
+        <v>114</v>
+      </c>
+      <c r="E67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73">
+        <v>90</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>118</v>
+      </c>
+      <c r="B83" t="s">
+        <v>119</v>
+      </c>
+      <c r="C83">
+        <v>20</v>
+      </c>
+      <c r="D83">
+        <v>100</v>
+      </c>
+      <c r="E83">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" t="s">
+        <v>142</v>
+      </c>
+      <c r="C86" t="s">
+        <v>114</v>
+      </c>
+      <c r="D86">
+        <v>100</v>
+      </c>
+      <c r="E86">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B88" t="s">
+        <v>131</v>
+      </c>
+      <c r="C88" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" t="s">
+        <v>114</v>
+      </c>
+      <c r="E88">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" t="s">
+        <v>131</v>
+      </c>
+      <c r="C96" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" t="s">
+        <v>114</v>
+      </c>
+      <c r="E96">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100" t="s">
+        <v>113</v>
+      </c>
+      <c r="C100" t="s">
+        <v>114</v>
+      </c>
+      <c r="D100" t="s">
+        <v>114</v>
+      </c>
+      <c r="E100">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
before second 99 hour
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="141">
   <si>
     <t>Golisopod</t>
   </si>
@@ -216,9 +216,6 @@
     <t>L55 Learn Hex 65+status</t>
   </si>
   <si>
-    <t>50 Forget Destiny Bond</t>
-  </si>
-  <si>
     <t>Ghost/Poison</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>Adamant/Sap Sipper</t>
   </si>
   <si>
-    <t>L44 Forget Flamethrower</t>
-  </si>
-  <si>
     <t>L49 Forget Scary</t>
   </si>
   <si>
@@ -282,9 +276,6 @@
     <t>TM26 Earthquack</t>
   </si>
   <si>
-    <t>L42 Forget Counter</t>
-  </si>
-  <si>
     <t>L47 Learn Earthquack</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>egg Close Combat</t>
   </si>
   <si>
-    <t>L43 Learn Thrash</t>
-  </si>
-  <si>
     <t>L49 Forget Pain Split</t>
   </si>
   <si>
@@ -321,12 +309,6 @@
     <t>Quiet/Schooling</t>
   </si>
   <si>
-    <t>L46 Forget Soak</t>
-  </si>
-  <si>
-    <t>L49 Forget Endeavor</t>
-  </si>
-  <si>
     <t>L54 Learn Hydro Pump</t>
   </si>
   <si>
@@ -454,6 +436,9 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>nmmnnnnnn</t>
   </si>
 </sst>
 </file>
@@ -911,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -929,22 +914,22 @@
     <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="D1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>405</v>
       </c>
@@ -973,12 +958,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -998,17 +983,14 @@
       <c r="I3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>530</v>
       </c>
@@ -1049,12 +1031,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>530</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1075,25 +1057,22 @@
         <v>24</v>
       </c>
       <c r="J5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>83</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="M5" t="s">
         <v>84</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="N5" t="s">
-        <v>86</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>500</v>
       </c>
@@ -1118,26 +1097,23 @@
       <c r="I6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="M6" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="N6" t="s">
         <v>89</v>
       </c>
-      <c r="L6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="O6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:14">
       <c r="F7" s="6"/>
       <c r="G7" s="25"/>
       <c r="H7" s="8"/>
@@ -1146,7 +1122,7 @@
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>464</v>
       </c>
@@ -1181,18 +1157,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>500</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E9">
         <v>33</v>
@@ -1210,27 +1186,24 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="M9" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="L9" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -1239,7 +1212,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E10">
         <v>39</v>
@@ -1256,80 +1229,77 @@
       <c r="I10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J10" t="s">
-        <v>101</v>
-      </c>
-      <c r="K10" t="s">
-        <v>102</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="N10" s="26" t="s">
+      <c r="J10" s="15" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="K10" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>500</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>600</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="5"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:14">
       <c r="A13" s="21">
         <v>530</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="22"/>
       <c r="F13" s="3"/>
       <c r="G13" s="5"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="L13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="21">
         <v>500</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="21"/>
       <c r="F14" s="3"/>
@@ -1337,7 +1307,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>490</v>
       </c>
@@ -1345,10 +1315,10 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="B16" s="10" t="s">
         <v>59</v>
       </c>
@@ -1356,6 +1326,9 @@
         <v>35</v>
       </c>
       <c r="D16" s="1"/>
+      <c r="K16" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="17" spans="3:8">
       <c r="C17" s="2" t="s">
@@ -1405,7 +1378,7 @@
       </c>
       <c r="D24" s="12"/>
       <c r="H24" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="3:8">
@@ -1442,16 +1415,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E1">
         <v>30</v>
@@ -1459,10 +1432,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C10">
         <v>60</v>
@@ -1476,16 +1449,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1493,10 +1466,10 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C31">
         <v>75</v>
@@ -1510,10 +1483,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C39">
         <v>60</v>
@@ -1527,13 +1500,13 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D41">
         <v>100</v>
@@ -1544,10 +1517,10 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C43">
         <v>50</v>
@@ -1561,16 +1534,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E44">
         <v>10</v>
@@ -1578,10 +1551,10 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C46">
         <v>60</v>
@@ -1595,10 +1568,10 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C48">
         <v>60</v>
@@ -1612,10 +1585,10 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C49">
         <v>40</v>
@@ -1632,7 +1605,7 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C54">
         <v>40</v>
@@ -1649,7 +1622,7 @@
         <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C55">
         <v>80</v>
@@ -1663,13 +1636,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D56">
         <v>100</v>
@@ -1680,10 +1653,10 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C57">
         <v>50</v>
@@ -1697,10 +1670,10 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C58">
         <v>60</v>
@@ -1717,7 +1690,7 @@
         <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C59">
         <v>60</v>
@@ -1731,10 +1704,10 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C62">
         <v>55</v>
@@ -1748,16 +1721,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B67" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C67">
         <v>70</v>
       </c>
       <c r="D67" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E67">
         <v>10</v>
@@ -1765,10 +1738,10 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B73" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C73">
         <v>90</v>
@@ -1779,10 +1752,10 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B83" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C83">
         <v>20</v>
@@ -1796,13 +1769,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C86" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D86">
         <v>100</v>
@@ -1813,16 +1786,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B88" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C88" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D88" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E88">
         <v>10</v>
@@ -1830,16 +1803,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B96" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C96" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D96" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E96">
         <v>20</v>
@@ -1847,16 +1820,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C100" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D100" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E100">
         <v>20</v>

</xml_diff>

<commit_message>
caught all kinds of natures Sync Abra
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="132">
   <si>
     <t>Golisopod</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Bug/Grass</t>
   </si>
   <si>
-    <t>L48  Liquidation 85</t>
-  </si>
-  <si>
     <t>TM28 Leech Life 80</t>
   </si>
   <si>
@@ -201,18 +198,12 @@
     <t>Bug/Fairy</t>
   </si>
   <si>
-    <t>L51 Learn</t>
-  </si>
-  <si>
     <t>405/500</t>
   </si>
   <si>
     <t>L61 Forget Nightmare</t>
   </si>
   <si>
-    <t>L55 Learn Hex 65+status</t>
-  </si>
-  <si>
     <t>Ghost/Poison</t>
   </si>
   <si>
@@ -270,9 +261,6 @@
     <t>TM26 Earthquack</t>
   </si>
   <si>
-    <t>L47 Learn Earthquack</t>
-  </si>
-  <si>
     <t>L55 Learn Mega Kick</t>
   </si>
   <si>
@@ -282,9 +270,6 @@
     <t>egg Close Combat</t>
   </si>
   <si>
-    <t>L49 Forget Pain Split</t>
-  </si>
-  <si>
     <t>L56 Learn Double Edge 120</t>
   </si>
   <si>
@@ -303,9 +288,6 @@
     <t>Quiet/Schooling</t>
   </si>
   <si>
-    <t>L54 Learn Hydro Pump</t>
-  </si>
-  <si>
     <t>TM13 Ice Beam 90</t>
   </si>
   <si>
@@ -430,9 +412,6 @@
   </si>
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <t>nmmnnnnnn</t>
   </si>
 </sst>
 </file>
@@ -892,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -906,7 +885,7 @@
     <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.44140625" bestFit="1" customWidth="1"/>
@@ -917,7 +896,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="D1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -948,16 +927,13 @@
       <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -977,11 +953,8 @@
       <c r="I3" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" t="s">
-        <v>63</v>
+      <c r="J3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1010,18 +983,15 @@
         <v>12</v>
       </c>
       <c r="J4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="M4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1030,7 +1000,7 @@
         <v>530</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1051,16 +1021,16 @@
         <v>24</v>
       </c>
       <c r="J5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>80</v>
-      </c>
-      <c r="K5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" t="s">
-        <v>82</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1088,20 +1058,17 @@
       <c r="I6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="K6" t="s">
-        <v>85</v>
+      <c r="J6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N6" t="s">
         <v>87</v>
+      </c>
+      <c r="M6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1118,7 +1085,7 @@
         <v>464</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1127,22 +1094,22 @@
         <v>39</v>
       </c>
       <c r="F8" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="I8" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="18" t="s">
+      <c r="J8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="J8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1150,13 +1117,13 @@
         <v>500</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E9">
         <v>33</v>
@@ -1173,25 +1140,22 @@
       <c r="I9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J9" t="s">
-        <v>88</v>
+      <c r="J9" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -1200,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E10">
         <v>39</v>
@@ -1218,13 +1182,10 @@
         <v>34</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="L10" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1232,10 +1193,10 @@
         <v>500</v>
       </c>
       <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
         <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="5"/>
@@ -1247,13 +1208,13 @@
         <v>600</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
         <v>76</v>
-      </c>
-      <c r="D12" t="s">
-        <v>79</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="5"/>
@@ -1265,29 +1226,26 @@
         <v>530</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="22"/>
       <c r="F13" s="3"/>
       <c r="G13" s="5"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="L13" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="21">
         <v>500</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D14" s="21"/>
       <c r="F14" s="3"/>
@@ -1303,19 +1261,19 @@
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="1"/>
       <c r="K16" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="3:8">
@@ -1366,7 +1324,7 @@
       </c>
       <c r="D24" s="12"/>
       <c r="H24" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="3:8">
@@ -1403,16 +1361,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E1">
         <v>30</v>
@@ -1420,10 +1378,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C10">
         <v>60</v>
@@ -1437,16 +1395,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1454,10 +1412,10 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C31">
         <v>75</v>
@@ -1471,10 +1429,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C39">
         <v>60</v>
@@ -1488,13 +1446,13 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D41">
         <v>100</v>
@@ -1505,10 +1463,10 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C43">
         <v>50</v>
@@ -1522,16 +1480,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E44">
         <v>10</v>
@@ -1539,10 +1497,10 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C46">
         <v>60</v>
@@ -1556,10 +1514,10 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C48">
         <v>60</v>
@@ -1573,10 +1531,10 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C49">
         <v>40</v>
@@ -1593,7 +1551,7 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C54">
         <v>40</v>
@@ -1610,7 +1568,7 @@
         <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C55">
         <v>80</v>
@@ -1624,13 +1582,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D56">
         <v>100</v>
@@ -1641,10 +1599,10 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C57">
         <v>50</v>
@@ -1658,10 +1616,10 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C58">
         <v>60</v>
@@ -1678,7 +1636,7 @@
         <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C59">
         <v>60</v>
@@ -1692,10 +1650,10 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C62">
         <v>55</v>
@@ -1709,16 +1667,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C67">
         <v>70</v>
       </c>
       <c r="D67" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E67">
         <v>10</v>
@@ -1726,10 +1684,10 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B73" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C73">
         <v>90</v>
@@ -1740,10 +1698,10 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B83" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C83">
         <v>20</v>
@@ -1757,13 +1715,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C86" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D86">
         <v>100</v>
@@ -1774,16 +1732,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B88" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C88" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D88" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E88">
         <v>10</v>
@@ -1791,16 +1749,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B96" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E96">
         <v>20</v>
@@ -1808,16 +1766,16 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C100" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D100" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E100">
         <v>20</v>

</xml_diff>